<commit_message>
remove meanthick, add 10_60
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="26">
   <si>
     <t>CIs</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>10_70</t>
+  </si>
+  <si>
+    <t>10_60</t>
   </si>
   <si>
     <t>15_65</t>
@@ -165,10 +168,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>33.0</v>
+        <v>29.0</v>
       </c>
       <c r="D2" t="n">
         <v>30.0</v>
@@ -182,10 +185,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>33.0</v>
+        <v>29.0</v>
       </c>
       <c r="D3" t="n">
         <v>30.0</v>
@@ -199,16 +202,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="n">
-        <v>39.0</v>
+        <v>29.0</v>
       </c>
       <c r="D4" t="n">
-        <v>35.0</v>
+        <v>44.0</v>
       </c>
       <c r="E4" t="n">
-        <v>16.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="5">
@@ -216,16 +219,16 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>39.0</v>
+        <v>29.0</v>
       </c>
       <c r="D5" t="n">
-        <v>35.0</v>
+        <v>44.0</v>
       </c>
       <c r="E5" t="n">
-        <v>16.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="6">
@@ -233,16 +236,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>39.0</v>
+        <v>38.0</v>
       </c>
       <c r="D6" t="n">
-        <v>44.0</v>
+        <v>35.0</v>
       </c>
       <c r="E6" t="n">
-        <v>19.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="7">
@@ -250,16 +253,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>39.0</v>
+        <v>38.0</v>
       </c>
       <c r="D7" t="n">
-        <v>44.0</v>
+        <v>35.0</v>
       </c>
       <c r="E7" t="n">
-        <v>19.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="8">
@@ -267,16 +270,16 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="n">
-        <v>39.0</v>
+        <v>38.0</v>
       </c>
       <c r="D8" t="n">
-        <v>30.0</v>
+        <v>44.0</v>
       </c>
       <c r="E8" t="n">
-        <v>15.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="9">
@@ -284,16 +287,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="n">
-        <v>39.0</v>
+        <v>38.0</v>
       </c>
       <c r="D9" t="n">
-        <v>30.0</v>
+        <v>44.0</v>
       </c>
       <c r="E9" t="n">
-        <v>15.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="10">
@@ -301,16 +304,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>49.0</v>
+        <v>38.0</v>
       </c>
       <c r="D10" t="n">
-        <v>35.0</v>
+        <v>30.0</v>
       </c>
       <c r="E10" t="n">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="11">
@@ -318,16 +321,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n">
-        <v>49.0</v>
+        <v>38.0</v>
       </c>
       <c r="D11" t="n">
-        <v>35.0</v>
+        <v>30.0</v>
       </c>
       <c r="E11" t="n">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="12">
@@ -335,16 +338,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="n">
-        <v>49.0</v>
+        <v>54.0</v>
       </c>
       <c r="D12" t="n">
-        <v>30.0</v>
+        <v>35.0</v>
       </c>
       <c r="E12" t="n">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="13">
@@ -352,16 +355,16 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="n">
-        <v>49.0</v>
+        <v>54.0</v>
       </c>
       <c r="D13" t="n">
-        <v>30.0</v>
+        <v>35.0</v>
       </c>
       <c r="E13" t="n">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="14">
@@ -369,16 +372,16 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>39.0</v>
+        <v>54.0</v>
       </c>
       <c r="D14" t="n">
-        <v>48.0</v>
+        <v>30.0</v>
       </c>
       <c r="E14" t="n">
-        <v>25.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="15">
@@ -386,16 +389,50 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>39.0</v>
+        <v>54.0</v>
       </c>
       <c r="D15" t="n">
-        <v>48.0</v>
+        <v>30.0</v>
       </c>
       <c r="E15" t="n">
-        <v>25.0</v>
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>23.0</v>
       </c>
     </row>
   </sheetData>
@@ -416,16 +453,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
@@ -433,13 +470,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="n">
-        <v>0.407060738893197</v>
+        <v>0.596532891672246</v>
       </c>
       <c r="E2"/>
     </row>
@@ -448,13 +485,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v>0.407060738893197</v>
+        <v>0.596532891672246</v>
       </c>
       <c r="E3"/>
     </row>
@@ -463,13 +500,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" t="n">
-        <v>0.315268537882078</v>
+        <v>0.889668168126462</v>
       </c>
       <c r="E4"/>
     </row>
@@ -478,13 +515,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" t="n">
-        <v>0.315268537882078</v>
+        <v>0.889668168126462</v>
       </c>
       <c r="E5"/>
     </row>
@@ -493,13 +530,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="n">
-        <v>0.546591748787477</v>
+        <v>0.297711053588368</v>
       </c>
       <c r="E6"/>
     </row>
@@ -508,13 +545,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" t="n">
-        <v>0.546591748787477</v>
+        <v>0.297711053588368</v>
       </c>
       <c r="E7"/>
     </row>
@@ -523,13 +560,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" t="n">
-        <v>0.339337408931477</v>
+        <v>0.656202142717386</v>
       </c>
       <c r="E8"/>
     </row>
@@ -538,13 +575,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D9" t="n">
-        <v>0.339337408931477</v>
+        <v>0.656202142717386</v>
       </c>
       <c r="E9"/>
     </row>
@@ -553,13 +590,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" t="n">
-        <v>0.379825961488246</v>
+        <v>0.351449297860668</v>
       </c>
       <c r="E10"/>
     </row>
@@ -568,13 +605,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11" t="n">
-        <v>0.379825961488246</v>
+        <v>0.351449297860668</v>
       </c>
       <c r="E11"/>
     </row>
@@ -583,13 +620,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D12" t="n">
-        <v>0.401631997162745</v>
+        <v>0.481135840878998</v>
       </c>
       <c r="E12"/>
     </row>
@@ -598,13 +635,13 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D13" t="n">
-        <v>0.401631997162745</v>
+        <v>0.481135840878998</v>
       </c>
       <c r="E13"/>
     </row>
@@ -613,13 +650,13 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" t="n">
-        <v>0.806383828403166</v>
+        <v>0.526225485744223</v>
       </c>
       <c r="E14"/>
     </row>
@@ -628,15 +665,45 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15" t="n">
-        <v>0.806383828403166</v>
+        <v>0.526225485744223</v>
       </c>
       <c r="E15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.801835629245378</v>
+      </c>
+      <c r="E16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.801835629245378</v>
+      </c>
+      <c r="E17"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -656,16 +723,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
@@ -673,16 +740,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" t="n">
-        <v>1.72630301661863E-9</v>
+        <v>4.10375653704166E-9</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
@@ -690,16 +757,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>1.72630301661863E-9</v>
+        <v>4.10375653704166E-9</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
@@ -707,16 +774,16 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>4.12834095141211E-11</v>
+        <v>7.13650084782703E-13</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5">
@@ -724,16 +791,16 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>4.12834095141211E-11</v>
+        <v>7.13650084782703E-13</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
@@ -741,16 +808,16 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
-        <v>1.66270735005133E-12</v>
+        <v>1.82101595113447E-11</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
@@ -758,16 +825,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" t="n">
-        <v>1.66270735005133E-12</v>
+        <v>1.82101595113447E-11</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -775,16 +842,16 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" t="n">
-        <v>1.28591623340606E-9</v>
+        <v>3.21708099720152E-13</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -792,16 +859,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" t="n">
-        <v>1.28591623340606E-9</v>
+        <v>3.21708099720152E-13</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
@@ -809,16 +876,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" t="n">
-        <v>9.35221447090469E-12</v>
+        <v>1.60666220915369E-9</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
@@ -826,16 +893,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>9.35221447090469E-12</v>
+        <v>1.60666220915369E-9</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
@@ -843,16 +910,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" t="n">
-        <v>3.2972371307521E-10</v>
+        <v>2.12474569676242E-12</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
@@ -860,16 +927,16 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" t="n">
-        <v>3.2972371307521E-10</v>
+        <v>2.12474569676242E-12</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
@@ -877,16 +944,16 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" t="n">
-        <v>7.90915729556192E-13</v>
+        <v>2.29305698617857E-10</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
@@ -894,16 +961,50 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" t="n">
-        <v>7.90915729556192E-13</v>
+        <v>2.29305698617857E-10</v>
       </c>
       <c r="E15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
         <v>20</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3.81018385428712E-12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3.81018385428712E-12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -924,16 +1025,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
@@ -941,13 +1042,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" t="n">
-        <v>0.188187381058959</v>
+        <v>0.388415617626828</v>
       </c>
       <c r="E2"/>
     </row>
@@ -956,13 +1057,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" t="n">
-        <v>0.188187381058959</v>
+        <v>0.388415617626828</v>
       </c>
       <c r="E3"/>
     </row>
@@ -971,13 +1072,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" t="n">
-        <v>0.157146819842407</v>
+        <v>0.0810962432818838</v>
       </c>
       <c r="E4"/>
     </row>
@@ -986,13 +1087,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" t="n">
-        <v>0.157146819842407</v>
+        <v>0.0810962432818838</v>
       </c>
       <c r="E5"/>
     </row>
@@ -1001,13 +1102,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0650887487548285</v>
+        <v>0.162609067399996</v>
       </c>
       <c r="E6"/>
     </row>
@@ -1016,13 +1117,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0650887487548285</v>
+        <v>0.162609067399996</v>
       </c>
       <c r="E7"/>
     </row>
@@ -1031,13 +1132,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" t="n">
-        <v>0.240035560396288</v>
+        <v>0.0626658993912413</v>
       </c>
       <c r="E8"/>
     </row>
@@ -1046,13 +1147,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" t="n">
-        <v>0.240035560396288</v>
+        <v>0.0626658993912413</v>
       </c>
       <c r="E9"/>
     </row>
@@ -1061,13 +1162,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" t="n">
-        <v>0.203983282086913</v>
+        <v>0.26278289541242</v>
       </c>
       <c r="E10"/>
     </row>
@@ -1076,13 +1177,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="n">
-        <v>0.203983282086913</v>
+        <v>0.26278289541242</v>
       </c>
       <c r="E11"/>
     </row>
@@ -1091,13 +1192,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D12" t="n">
-        <v>0.302825700602156</v>
+        <v>0.160211356612228</v>
       </c>
       <c r="E12"/>
     </row>
@@ -1106,13 +1207,13 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" t="n">
-        <v>0.302825700602156</v>
+        <v>0.160211356612228</v>
       </c>
       <c r="E13"/>
     </row>
@@ -1121,13 +1222,13 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0605525362063025</v>
+        <v>0.262048873727635</v>
       </c>
       <c r="E14"/>
     </row>
@@ -1136,15 +1237,45 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0605525362063025</v>
+        <v>0.262048873727635</v>
       </c>
       <c r="E15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.144592022351181</v>
+      </c>
+      <c r="E16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.144592022351181</v>
+      </c>
+      <c r="E17"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1164,16 +1295,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
@@ -1181,13 +1312,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
-        <v>0.203449316616009</v>
+        <v>0.138714406846369</v>
       </c>
       <c r="E2"/>
     </row>
@@ -1196,13 +1327,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3" t="n">
-        <v>0.203449316616009</v>
+        <v>0.138714406846369</v>
       </c>
       <c r="E3"/>
     </row>
@@ -1211,13 +1342,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="n">
-        <v>0.447822477084724</v>
+        <v>0.13511353342347</v>
       </c>
       <c r="E4"/>
     </row>
@@ -1226,13 +1357,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
-        <v>0.447822477084724</v>
+        <v>0.13511353342347</v>
       </c>
       <c r="E5"/>
     </row>
@@ -1241,13 +1372,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" t="n">
-        <v>0.225387814782236</v>
+        <v>0.306386177402415</v>
       </c>
       <c r="E6"/>
     </row>
@@ -1256,13 +1387,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" t="n">
-        <v>0.225387814782236</v>
+        <v>0.306386177402415</v>
       </c>
       <c r="E7"/>
     </row>
@@ -1271,13 +1402,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" t="n">
-        <v>0.187952382154039</v>
+        <v>0.158829686602599</v>
       </c>
       <c r="E8"/>
     </row>
@@ -1286,13 +1417,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="n">
-        <v>0.187952382154039</v>
+        <v>0.158829686602599</v>
       </c>
       <c r="E9"/>
     </row>
@@ -1301,13 +1432,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" t="n">
-        <v>0.316170367389708</v>
+        <v>0.157972301952884</v>
       </c>
       <c r="E10"/>
     </row>
@@ -1316,13 +1447,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" t="n">
-        <v>0.316170367389708</v>
+        <v>0.157972301952884</v>
       </c>
       <c r="E11"/>
     </row>
@@ -1331,13 +1462,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" t="n">
-        <v>0.115465260430079</v>
+        <v>0.143690569286009</v>
       </c>
       <c r="E12"/>
     </row>
@@ -1346,13 +1477,13 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" t="n">
-        <v>0.115465260430079</v>
+        <v>0.143690569286009</v>
       </c>
       <c r="E13"/>
     </row>
@@ -1361,13 +1492,13 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" t="n">
-        <v>0.318815452981043</v>
+        <v>0.0659691689837428</v>
       </c>
       <c r="E14"/>
     </row>
@@ -1376,15 +1507,45 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" t="n">
-        <v>0.318815452981043</v>
+        <v>0.0659691689837428</v>
       </c>
       <c r="E15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.164413300020516</v>
+      </c>
+      <c r="E16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.164413300020516</v>
+      </c>
+      <c r="E17"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1404,16 +1565,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
@@ -1421,13 +1582,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" t="n">
-        <v>0.43174442274246</v>
+        <v>0.871494778760503</v>
       </c>
       <c r="E2"/>
     </row>
@@ -1436,13 +1597,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" t="n">
-        <v>0.43174442274246</v>
+        <v>0.871494778760503</v>
       </c>
       <c r="E3"/>
     </row>
@@ -1451,13 +1612,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" t="n">
-        <v>0.672759076964209</v>
+        <v>0.911084729800738</v>
       </c>
       <c r="E4"/>
     </row>
@@ -1466,13 +1627,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" t="n">
-        <v>0.672759076964209</v>
+        <v>0.911084729800738</v>
       </c>
       <c r="E5"/>
     </row>
@@ -1481,13 +1642,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
-        <v>0.849715084901025</v>
+        <v>0.714885746184298</v>
       </c>
       <c r="E6"/>
     </row>
@@ -1496,13 +1657,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" t="n">
-        <v>0.849715084901025</v>
+        <v>0.714885746184298</v>
       </c>
       <c r="E7"/>
     </row>
@@ -1511,13 +1672,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" t="n">
-        <v>0.722760013823793</v>
+        <v>0.850495139762909</v>
       </c>
       <c r="E8"/>
     </row>
@@ -1526,13 +1687,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" t="n">
-        <v>0.722760013823793</v>
+        <v>0.850495139762909</v>
       </c>
       <c r="E9"/>
     </row>
@@ -1541,13 +1702,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" t="n">
-        <v>0.793413261720042</v>
+        <v>0.745014114133694</v>
       </c>
       <c r="E10"/>
     </row>
@@ -1556,13 +1717,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D11" t="n">
-        <v>0.793413261720042</v>
+        <v>0.745014114133694</v>
       </c>
       <c r="E11"/>
     </row>
@@ -1571,13 +1732,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" t="n">
-        <v>0.834011116428233</v>
+        <v>0.687074028485019</v>
       </c>
       <c r="E12"/>
     </row>
@@ -1586,13 +1747,13 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D13" t="n">
-        <v>0.834011116428233</v>
+        <v>0.687074028485019</v>
       </c>
       <c r="E13"/>
     </row>
@@ -1601,13 +1762,13 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D14" t="n">
-        <v>0.90817581736484</v>
+        <v>0.721251933108614</v>
       </c>
       <c r="E14"/>
     </row>
@@ -1616,15 +1777,45 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D15" t="n">
-        <v>0.90817581736484</v>
+        <v>0.721251933108614</v>
       </c>
       <c r="E15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.938065697617005</v>
+      </c>
+      <c r="E16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.938065697617005</v>
+      </c>
+      <c r="E17"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1644,16 +1835,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
@@ -1661,13 +1852,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" t="n">
-        <v>0.794161368855019</v>
+        <v>0.946909263377894</v>
       </c>
       <c r="E2"/>
     </row>
@@ -1676,13 +1867,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>0.794161368855019</v>
+        <v>0.946909263377894</v>
       </c>
       <c r="E3"/>
     </row>
@@ -1691,13 +1882,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>0.643134890104883</v>
+        <v>0.367517556229913</v>
       </c>
       <c r="E4"/>
     </row>
@@ -1706,13 +1897,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" t="n">
-        <v>0.643134890104883</v>
+        <v>0.367517556229913</v>
       </c>
       <c r="E5"/>
     </row>
@@ -1721,13 +1912,13 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" t="n">
-        <v>0.46947382014926</v>
+        <v>0.639514965523343</v>
       </c>
       <c r="E6"/>
     </row>
@@ -1736,13 +1927,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>0.46947382014926</v>
+        <v>0.639514965523343</v>
       </c>
       <c r="E7"/>
     </row>
@@ -1751,13 +1942,13 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" t="n">
-        <v>0.945457181154344</v>
+        <v>0.376107296387777</v>
       </c>
       <c r="E8"/>
     </row>
@@ -1766,13 +1957,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" t="n">
-        <v>0.945457181154344</v>
+        <v>0.376107296387777</v>
       </c>
       <c r="E9"/>
     </row>
@@ -1781,13 +1972,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" t="n">
-        <v>0.625102723624199</v>
+        <v>0.941249762651856</v>
       </c>
       <c r="E10"/>
     </row>
@@ -1796,13 +1987,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11" t="n">
-        <v>0.625102723624199</v>
+        <v>0.941249762651856</v>
       </c>
       <c r="E11"/>
     </row>
@@ -1811,13 +2002,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9426175982002</v>
+        <v>0.626802529674606</v>
       </c>
       <c r="E12"/>
     </row>
@@ -1826,13 +2017,13 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9426175982002</v>
+        <v>0.626802529674606</v>
       </c>
       <c r="E13"/>
     </row>
@@ -1841,13 +2032,13 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D14" t="n">
-        <v>0.457707911225385</v>
+        <v>0.916894761907062</v>
       </c>
       <c r="E14"/>
     </row>
@@ -1856,15 +2047,45 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" t="n">
-        <v>0.457707911225385</v>
+        <v>0.916894761907062</v>
       </c>
       <c r="E15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.599733397075688</v>
+      </c>
+      <c r="E16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.599733397075688</v>
+      </c>
+      <c r="E17"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>